<commit_message>
corrected missing embodied emission file
</commit_message>
<xml_diff>
--- a/data/scenarios.xlsx
+++ b/data/scenarios.xlsx
@@ -436,7 +436,7 @@
   <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +488,7 @@
         <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H2" t="s">
         <v>11</v>

</xml_diff>